<commit_message>
ubacen graduate i spojen sa excelom
</commit_message>
<xml_diff>
--- a/course_assignments.xlsx
+++ b/course_assignments.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F293"/>
+  <dimension ref="A1:F333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B F2.5</t>
+          <t>B F1.25 Computer Lab</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>B F1.2 - Class/ECON Lab</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1173,7 +1173,7 @@
         <v>14</v>
       </c>
       <c r="E27" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>B F1.2 - Class/ECON Lab</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1201,7 +1201,7 @@
         <v>11</v>
       </c>
       <c r="E28" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>B F1.17</t>
+          <t>B F1.35 FBA Conference Room</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>A F1.18 - Computer Lab</t>
+          <t>A B.2 - EE Lab</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>B F2.15 - Amphitheater II</t>
+          <t>B F1.23 - Amphitheater I</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>B F2.15 - Amphitheater II</t>
+          <t>B F1.23 - Amphitheater I</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>B F2.15 - Amphitheater II</t>
+          <t>B F1.23 - Amphitheater I</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>A B.2 - EE Lab</t>
+          <t>A F1.3 - Computer Lab</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>RC.G1 - GBE Laboratory I</t>
+          <t>RC.G4 - GBE IV</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>A B.13 - Class/PSY Lab</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2769,7 +2769,7 @@
         <v>12</v>
       </c>
       <c r="E84" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio</t>
+          <t>A F1.18 - Computer Lab</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>B F1.2 - Class/ECON Lab</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3373,7 +3373,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>A B.2 - EE Lab</t>
+          <t>A F1.18 - Computer Lab</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>B F2.8</t>
+          <t>A B.1 - VACD Multimedia Studio</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>B F1.2 - Class/ECON Lab</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3637,7 +3637,7 @@
         <v>5</v>
       </c>
       <c r="E115" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>B F1.2 - Class/ECON Lab</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>A F3.10 - Architecture Classroom</t>
+          <t>A F1.17</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>A F3.8 - Big Architecture Studio</t>
+          <t>A F1.18 - Computer Lab</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>B F1.10 Class/ART Studio</t>
+          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4437,7 +4437,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>B F2.16</t>
+          <t>B F2.17</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>A F1.18 - Computer Lab</t>
+          <t>A F2.8 - Drawing Studio</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>B F2.5</t>
+          <t>B F1.9</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -5053,7 +5053,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>B F1.10 Class/ART Studio</t>
+          <t>A B.16 - VACD Drawing Studio</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>B F1.17</t>
+          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5389,7 +5389,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio</t>
+          <t>A F1.3 - Computer Lab</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
+          <t>B F1.10 Class/ART Studio</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -5641,7 +5641,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>B F1.22</t>
+          <t>B F1.35 FBA Conference Room</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -5669,7 +5669,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>B F2.17</t>
+          <t>B F2.16</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>B F2.15 - Amphitheater II</t>
+          <t>B F1.23 - Amphitheater I</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>B F1.23 - Amphitheater I</t>
+          <t>B F2.15 - Amphitheater II</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -6335,7 +6335,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>B F1.8</t>
+          <t>B F2.6</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -6531,7 +6531,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
+          <t>B F1.22</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -6783,7 +6783,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>A F1.4 - Class/Laboratory</t>
+          <t>A B.8 - Fabrication Lab</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -6923,7 +6923,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>B F1.24 (MAC Studio)</t>
+          <t>B F1.16</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -7287,7 +7287,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>A B.13 - Class/PSY Lab</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -7299,7 +7299,7 @@
         <v>5</v>
       </c>
       <c r="E246" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F246" t="inlineStr">
         <is>
@@ -7483,7 +7483,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>A B.13 - Class/PSY Lab</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -7495,7 +7495,7 @@
         <v>8</v>
       </c>
       <c r="E253" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F253" t="inlineStr">
         <is>
@@ -7623,7 +7623,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>B F1.17</t>
+          <t>B F1.22</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -7679,7 +7679,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>B F2.14</t>
+          <t>B F1.16</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
+          <t>A B.16 - VACD Drawing Studio</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -8379,7 +8379,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>B F2.17</t>
+          <t>B F2.16</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -8618,6 +8618,1126 @@
         <v>25</v>
       </c>
       <c r="F293" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>ARCH510.1</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Wed. 17:00-18:50</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>9</v>
+      </c>
+      <c r="E294" t="n">
+        <v>12</v>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>ARCH517.1</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Tue. 10:00-15:50</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>15</v>
+      </c>
+      <c r="E295" t="n">
+        <v>18</v>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>ARCH569.1</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Thu. 17:00-18:50</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>5</v>
+      </c>
+      <c r="E296" t="n">
+        <v>12</v>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>ARCH570.1</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-18:50</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>5</v>
+      </c>
+      <c r="E297" t="n">
+        <v>12</v>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>BIO513.1</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>A F2.16 - Architecture Studio</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Fri. 14:00-16:50</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>9</v>
+      </c>
+      <c r="E298" t="n">
+        <v>20</v>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>BIO514.1</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Wed. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>6</v>
+      </c>
+      <c r="E299" t="n">
+        <v>18</v>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>BIO518.1</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>A F2.16 - Architecture Studio</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Thu. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>9</v>
+      </c>
+      <c r="E300" t="n">
+        <v>20</v>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>BIO604.1</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>A F2.16 - Architecture Studio</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Wed. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>3</v>
+      </c>
+      <c r="E301" t="n">
+        <v>20</v>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>BIO646.1</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>A F2.16 - Architecture Studio</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>3</v>
+      </c>
+      <c r="E302" t="n">
+        <v>20</v>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>BUS602.1</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Fri. 14:00-16:50</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>2</v>
+      </c>
+      <c r="E303" t="n">
+        <v>18</v>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>CS509.1</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>13</v>
+      </c>
+      <c r="E304" t="n">
+        <v>18</v>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>CS511.1</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>RC1.3 - GSM and Network Laboratories</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Thu. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>15</v>
+      </c>
+      <c r="E305" t="n">
+        <v>20</v>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>ECON506.1</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>A F3.8 - Big Architecture Studio</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Thu. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>2</v>
+      </c>
+      <c r="E306" t="n">
+        <v>25</v>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>ECON601.1</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>A F1.3 - Computer Lab</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Thu. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>2</v>
+      </c>
+      <c r="E307" t="n">
+        <v>25</v>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>EDU583.1</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Thu. 16:00-18:50</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>7</v>
+      </c>
+      <c r="E308" t="n">
+        <v>12</v>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>ELT562.1</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>A F2.16 - Architecture Studio</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Fri. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>9</v>
+      </c>
+      <c r="E309" t="n">
+        <v>20</v>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>ELT565.1</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>B F1.2 - Class/ECON Lab</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Thu. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>9</v>
+      </c>
+      <c r="E310" t="n">
+        <v>20</v>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>ELT599.1</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Mon. 17:00-17:50</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>4</v>
+      </c>
+      <c r="E311" t="n">
+        <v>12</v>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>ELT660.1</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Fri. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>1</v>
+      </c>
+      <c r="E312" t="n">
+        <v>18</v>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>ELT670.1</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Thu. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>1</v>
+      </c>
+      <c r="E313" t="n">
+        <v>12</v>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>IBF507.1</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>A B.2 - EE Lab</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Wed. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>22</v>
+      </c>
+      <c r="E314" t="n">
+        <v>25</v>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>IBF562.1</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>A F1.4 - Class/Laboratory</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>27</v>
+      </c>
+      <c r="E315" t="n">
+        <v>30</v>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>IE502.1</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Fri. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>4</v>
+      </c>
+      <c r="E316" t="n">
+        <v>12</v>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>IR520.1</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>B F1.2 - Class/ECON Lab</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>3</v>
+      </c>
+      <c r="E317" t="n">
+        <v>20</v>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>IR651.1</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>A F2.16 - Architecture Studio</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Mon. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>2</v>
+      </c>
+      <c r="E318" t="n">
+        <v>20</v>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>IR652.1</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>RC1.4 - Computer Laboratory</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>1</v>
+      </c>
+      <c r="E319" t="n">
+        <v>20</v>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>LAW530.1</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Fri. 18:00-20:50</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>4</v>
+      </c>
+      <c r="E320" t="n">
+        <v>12</v>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>MBA525.1</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>A B.2 - EE Lab</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Fri. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>21</v>
+      </c>
+      <c r="E321" t="n">
+        <v>25</v>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>MBA535.1</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>A B.1 - VACD Multimedia Studio</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Mon. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>31</v>
+      </c>
+      <c r="E322" t="n">
+        <v>35</v>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>MBA581.1</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>RC1.3 - GSM and Network Laboratories</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Wed. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>6</v>
+      </c>
+      <c r="E323" t="n">
+        <v>20</v>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>ME510.1</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>A F1.3 - Computer Lab</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>3</v>
+      </c>
+      <c r="E324" t="n">
+        <v>25</v>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>PSY519.1</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>RC1.3 - GSM and Network Laboratories</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>7</v>
+      </c>
+      <c r="E325" t="n">
+        <v>20</v>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>PSY524.1</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Mon. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>4</v>
+      </c>
+      <c r="E326" t="n">
+        <v>18</v>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>PSY529.1</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>RC1.4 - Computer Laboratory</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Thu. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>6</v>
+      </c>
+      <c r="E327" t="n">
+        <v>20</v>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>SOC503.1</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>B F1.2 - Class/ECON Lab</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Wed. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>3</v>
+      </c>
+      <c r="E328" t="n">
+        <v>20</v>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>SPS509.1</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Mon. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>1</v>
+      </c>
+      <c r="E329" t="n">
+        <v>12</v>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>SPS603.1</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>Wed. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>1</v>
+      </c>
+      <c r="E330" t="n">
+        <v>12</v>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>VA502.1</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>Thu. 18:00-20:50</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>7</v>
+      </c>
+      <c r="E331" t="n">
+        <v>12</v>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>VA517.1</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Tue. 17:00-19:50</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>7</v>
+      </c>
+      <c r="E332" t="n">
+        <v>12</v>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>VA519.1</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Mon. 18:00-20:50</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>7</v>
+      </c>
+      <c r="E333" t="n">
+        <v>12</v>
+      </c>
+      <c r="F333" t="inlineStr">
         <is>
           <t>Assigned</t>
         </is>

</xml_diff>

<commit_message>
ubaceni ens207 i ens209
</commit_message>
<xml_diff>
--- a/course_assignments.xlsx
+++ b/course_assignments.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F333"/>
+  <dimension ref="A1:F334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B F1.25 Computer Lab</t>
+          <t>B F2.5</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A B.13 - Class/PSY Lab</t>
+          <t>A F2.16 - Architecture Studio</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -837,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>A F2.16 - Architecture Studio</t>
+          <t>A B.13 - Class/PSY Lab</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1453,7 +1453,7 @@
         <v>6</v>
       </c>
       <c r="E37" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>A B.2 - EE Lab</t>
+          <t>A F3.8 - Big Architecture Studio</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>B F1.23 - Amphitheater I</t>
+          <t>B F2.15 - Amphitheater II</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>RC.G5 - ME Laboratory</t>
+          <t>A F1.25</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>A F1.3 - Computer Lab</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2769,7 +2769,7 @@
         <v>12</v>
       </c>
       <c r="E84" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>B F1.2 - Class/ECON Lab</t>
+          <t>RC1.4 - Computer Laboratory</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3373,7 +3373,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>A B.2 - EE Lab</t>
+          <t>A F1.18 - Computer Lab</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3877,7 +3877,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>RC1.3 - GSM and Network Laboratories</t>
+          <t>B F1.2 - Class/ECON Lab</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4068,24 +4068,24 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>ENS207-6.1</t>
+          <t>ENS209</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>A F1.25</t>
+          <t>B F1.16</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Fri. 09:00-09:50</t>
+          <t>Tue. 17:00-19:50</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E131" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>A F1.25</t>
+          <t>A F1.17</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>A B.16 - VACD Drawing Studio</t>
+          <t>B F1.10 Class/ART Studio</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4549,7 +4549,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>A F2.3</t>
+          <t>A F3.7 - Small Architecture Studio &amp; A F3.10 - Architecture Classroom</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4577,7 +4577,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>B F2.15 - Amphitheater II</t>
+          <t>B F1.23 - Amphitheater I</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>A B.2 - EE Lab</t>
+          <t>A F2.8 - Drawing Studio</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4969,7 +4969,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
+          <t>B F1.10 Class/ART Studio</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>B F1.9</t>
+          <t>B F1.25 Computer Lab</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -5053,7 +5053,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>B F1.10 Class/ART Studio</t>
+          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>B F1.17</t>
+          <t>B F1.35 FBA Conference Room</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5305,7 +5305,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>RC1.3 - GSM and Network Laboratories</t>
+          <t>RC1.4 - Computer Laboratory</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -5389,7 +5389,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>A F1.3 - Computer Lab</t>
+          <t>A B.2 - EE Lab</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -5529,7 +5529,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>A F3.7 - Small Architecture Studio</t>
+          <t>A F1.4 - Class/Laboratory</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>B F1.17</t>
+          <t>B F1.10 Class/ART Studio</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -5641,7 +5641,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>B F1.22</t>
+          <t>B F1.35 FBA Conference Room</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -5669,7 +5669,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>B F2.16</t>
+          <t>B F2.17</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -5893,7 +5893,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>B F1.23 - Amphitheater I</t>
+          <t>B F2.15 - Amphitheater II</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>B F2.15 - Amphitheater II</t>
+          <t>B F1.23 - Amphitheater I</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>B F2.15 - Amphitheater II</t>
+          <t>B F1.23 - Amphitheater I</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -6139,7 +6139,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>A F3.7 - Small Architecture Studio</t>
+          <t>A F1.4 - Class/Laboratory</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -6335,7 +6335,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>A F1.11</t>
+          <t>A F1.10</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -6531,7 +6531,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>B F1.22</t>
+          <t>B F1.10 Class/ART Studio</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -6671,7 +6671,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>B F1.9</t>
+          <t>B F2.5</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -6923,7 +6923,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>B F1.24 (MAC Studio)</t>
+          <t>B F1.16</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
+          <t>B F1.10 Class/ART Studio</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -7819,7 +7819,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>A B.1 - VACD Multimedia Studio</t>
+          <t>B F2.2</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -8351,7 +8351,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>B F1.2 - Class/ECON Lab</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>A F3.8 - Big Architecture Studio</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -8923,7 +8923,7 @@
         <v>13</v>
       </c>
       <c r="E304" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F304" t="inlineStr">
         <is>
@@ -8939,7 +8939,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>A B.2 - EE Lab</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -8951,7 +8951,7 @@
         <v>15</v>
       </c>
       <c r="E305" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F305" t="inlineStr">
         <is>
@@ -8967,7 +8967,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>RC1.3 - GSM and Network Laboratories</t>
+          <t>A F3.8 - Big Architecture Studio</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -8979,7 +8979,7 @@
         <v>2</v>
       </c>
       <c r="E306" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F306" t="inlineStr">
         <is>
@@ -8995,7 +8995,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -9007,7 +9007,7 @@
         <v>2</v>
       </c>
       <c r="E307" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F307" t="inlineStr">
         <is>
@@ -9191,7 +9191,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>A F1.3 - Computer Lab</t>
+          <t>A B.2 - EE Lab</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -9331,7 +9331,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>RC1.3 - GSM and Network Laboratories</t>
+          <t>RC1.4 - Computer Laboratory</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>A F2.8 - Drawing Studio</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -9511,7 +9511,7 @@
         <v>7</v>
       </c>
       <c r="E325" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F325" t="inlineStr">
         <is>
@@ -9527,7 +9527,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>A B.13 - Class/PSY Lab</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -9539,7 +9539,7 @@
         <v>4</v>
       </c>
       <c r="E326" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F326" t="inlineStr">
         <is>
@@ -9555,7 +9555,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio</t>
+          <t>RC1.4 - Computer Laboratory</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -9567,7 +9567,7 @@
         <v>6</v>
       </c>
       <c r="E327" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F327" t="inlineStr">
         <is>
@@ -9611,7 +9611,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>A B.13 - Class/PSY Lab</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -9623,7 +9623,7 @@
         <v>1</v>
       </c>
       <c r="E329" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F329" t="inlineStr">
         <is>
@@ -9695,7 +9695,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -9707,7 +9707,7 @@
         <v>7</v>
       </c>
       <c r="E332" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F332" t="inlineStr">
         <is>
@@ -9738,6 +9738,34 @@
         <v>12</v>
       </c>
       <c r="F333" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>ENS207</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>B F2.16</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Fri. 09:00-09:50</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>71</v>
+      </c>
+      <c r="E334" t="n">
+        <v>80</v>
+      </c>
+      <c r="F334" t="inlineStr">
         <is>
           <t>Assigned</t>
         </is>

</xml_diff>

<commit_message>
dodana 4 graduate courses
</commit_message>
<xml_diff>
--- a/course_assignments.xlsx
+++ b/course_assignments.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F333"/>
+  <dimension ref="A1:F337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B F1.9</t>
+          <t>B F2.5</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>B F2.8</t>
+          <t>B F2.2</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>A B.2 - EE Lab</t>
+          <t>A F1.3 - Computer Lab</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>B F1.23 - Amphitheater I</t>
+          <t>B F2.15 - Amphitheater II</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>B F1.23 - Amphitheater I</t>
+          <t>B F2.15 - Amphitheater II</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>A F1.23</t>
+          <t>RC.G4 - GBE IV</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>A F1.3 - Computer Lab</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2741,7 +2741,7 @@
         <v>12</v>
       </c>
       <c r="E83" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>A F1.3 - Computer Lab</t>
+          <t>A B.13 - Class/PSY Lab</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2853,7 +2853,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>A F1.4 - Class/Laboratory</t>
+          <t>A B.8 - Fabrication Lab</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>A F1.3 - Computer Lab</t>
+          <t>A B.2 - EE Lab</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>B F1.2 - Class/ECON Lab</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3317,7 +3317,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3373,7 +3373,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>B F2.2</t>
+          <t>A B.1 - VACD Multimedia Studio</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>RC1.3 - GSM and Network Laboratories</t>
+          <t>B F1.2 - Class/ECON Lab</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4129,7 +4129,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>A F1.23</t>
+          <t>A F3.10 - Architecture Classroom</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>A B.16 - VACD Drawing Studio</t>
+          <t>B F1.35 FBA Conference Room</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4409,7 +4409,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>B F2.17</t>
+          <t>B F2.16</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4689,7 +4689,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>A F1.3 - Computer Lab</t>
+          <t>A B.2 - EE Lab</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>A B.13 - Class/PSY Lab</t>
+          <t>A F2.16 - Architecture Studio</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -4813,7 +4813,7 @@
         <v>8</v>
       </c>
       <c r="E157" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>B F1.22</t>
+          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>B F1.17</t>
+          <t>A B.16 - VACD Drawing Studio</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -5193,7 +5193,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>B F1.17</t>
+          <t>B F1.35 FBA Conference Room</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5501,7 +5501,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>A B.8 - Fabrication Lab</t>
+          <t>A F3.7 - Small Architecture Studio</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -5529,7 +5529,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>A B.16 - VACD Drawing Studio</t>
+          <t>B F1.22</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5641,7 +5641,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>B F2.16</t>
+          <t>B F2.17</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -5943,7 +5943,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>B F2.15 - Amphitheater II</t>
+          <t>B F1.23 - Amphitheater I</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -6111,7 +6111,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>A F3.7 - Small Architecture Studio</t>
+          <t>RC1.5 - Electronic Laboratory</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>A F1.10</t>
+          <t>A F1.26</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -6503,7 +6503,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>B F1.22</t>
+          <t>A F2.8 - Drawing Studio &amp; A F2.16 - Architecture Studio</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -6895,7 +6895,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>B F1.16</t>
+          <t>B F1.24 (MAC Studio)</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -7007,7 +7007,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>A F2.16 - Architecture Studio</t>
+          <t>A B.2 - EE Lab</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -7019,7 +7019,7 @@
         <v>14</v>
       </c>
       <c r="E236" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F236" t="inlineStr">
         <is>
@@ -7595,7 +7595,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>B F1.22</t>
+          <t>A B.16 - VACD Drawing Studio</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -7763,7 +7763,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>B F1.17</t>
+          <t>B F1.10 Class/ART Studio</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>A B.1 - VACD Multimedia Studio</t>
+          <t>B F2.2</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -8239,7 +8239,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>A F1.18 - Computer Lab</t>
+          <t>A B.2 - EE Lab</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -8323,7 +8323,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>RC1.3 - GSM and Network Laboratories</t>
+          <t>B F1.2 - Class/ECON Lab</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -8883,7 +8883,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>A F3.8 - Big Architecture Studio</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -8895,7 +8895,7 @@
         <v>13</v>
       </c>
       <c r="E303" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F303" t="inlineStr">
         <is>
@@ -8911,7 +8911,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>RC1.4 - Computer Laboratory</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -8923,7 +8923,7 @@
         <v>15</v>
       </c>
       <c r="E304" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F304" t="inlineStr">
         <is>
@@ -9163,7 +9163,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>A B.2 - EE Lab</t>
+          <t>A F1.3 - Computer Lab</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -9303,7 +9303,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>A B.13 - Class/PSY Lab</t>
+          <t>RC1.4 - Computer Laboratory</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -9315,7 +9315,7 @@
         <v>1</v>
       </c>
       <c r="E318" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F318" t="inlineStr">
         <is>
@@ -9443,7 +9443,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>RC1.3 - GSM and Network Laboratories</t>
+          <t>A B.13 - Class/PSY Lab</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -9455,7 +9455,7 @@
         <v>3</v>
       </c>
       <c r="E323" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F323" t="inlineStr">
         <is>
@@ -9471,7 +9471,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>RC1.4 - Computer Laboratory</t>
+          <t>A F2.8 - Drawing Studio</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -9483,7 +9483,7 @@
         <v>7</v>
       </c>
       <c r="E324" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F324" t="inlineStr">
         <is>
@@ -9499,7 +9499,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>A B.13 - Class/PSY Lab</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -9511,7 +9511,7 @@
         <v>4</v>
       </c>
       <c r="E325" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F325" t="inlineStr">
         <is>
@@ -9527,7 +9527,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>A F2.8 - Drawing Studio</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -9539,7 +9539,7 @@
         <v>6</v>
       </c>
       <c r="E326" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F326" t="inlineStr">
         <is>
@@ -9583,7 +9583,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>A B.13 - Class/PSY Lab</t>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -9595,7 +9595,7 @@
         <v>1</v>
       </c>
       <c r="E328" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F328" t="inlineStr">
         <is>
@@ -9667,7 +9667,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>B F2.27 Creative Writing and Translation Studio</t>
+          <t>RC1.3 - GSM and Network Laboratories</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -9679,7 +9679,7 @@
         <v>7</v>
       </c>
       <c r="E331" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F331" t="inlineStr">
         <is>
@@ -9723,7 +9723,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>B F2.17</t>
+          <t>B F2.16</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -9738,6 +9738,118 @@
         <v>80</v>
       </c>
       <c r="F333" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>CS600.1</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Tue. 17:00 - 19:50</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>3</v>
+      </c>
+      <c r="E334" t="n">
+        <v>12</v>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>EE603.1</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Mon. 15:00 - 17:50</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>3</v>
+      </c>
+      <c r="E335" t="n">
+        <v>12</v>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>ME605.1</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>A B.13 - Class/PSY Lab</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Wed. 17:00 - 19:50</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>3</v>
+      </c>
+      <c r="E336" t="n">
+        <v>12</v>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>ME580.1</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>B F2.27 Creative Writing and Translation Studio</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>Mon. 17:00 - 19:50</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>13</v>
+      </c>
+      <c r="E337" t="n">
+        <v>18</v>
+      </c>
+      <c r="F337" t="inlineStr">
         <is>
           <t>Assigned</t>
         </is>

</xml_diff>